<commit_message>
testes de upload e inserção de dados direto no bd
feito import de carros, registros e motoristas, insert de registros, teste de pesquisa no bd
</commit_message>
<xml_diff>
--- a/planilhas/carros.xlsx
+++ b/planilhas/carros.xlsx
@@ -8,17 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\VoidDash\planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689F05E5-506D-4424-BB5E-2386971602A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA3758F-EC1E-4FB5-B020-0E649EFAE77D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -612,11 +623,12 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>

</xml_diff>